<commit_message>
Update for LPF BOM
Update for LPF BOM
</commit_message>
<xml_diff>
--- a/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Control_Board_BOM_V1.00_01-14-24.xlsx
+++ b/K9HZ_LPF_Module/K9HZ_LPF_V1.00_BOMs/K9HZ_LPF-Control_Board_BOM_V1.00_01-14-24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\T41\K9HZ_LFP_Module\K9HZ_LPF_V1.00_BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\T41\K9HZ_LPF_Module\K9HZ_LPF_V1.00_BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8724FD7C-F3D1-4935-AA62-FD41A524851E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8135943D-06DC-4C70-BC13-2F7A19655FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,9 +421,6 @@
     <t>584-AD8307ARZ-R7</t>
   </si>
   <si>
-    <t>70-ILSB1206ER220K</t>
-  </si>
-  <si>
     <t>81-1264EY-100MP3</t>
   </si>
   <si>
@@ -445,9 +442,6 @@
     <t>A-1304</t>
   </si>
   <si>
-    <t>22uH SMD 1206 Inductor</t>
-  </si>
-  <si>
     <t>10uH 20% Power Inductor</t>
   </si>
   <si>
@@ -479,6 +473,12 @@
   </si>
   <si>
     <t>71-CRCW1206-52.3-E3</t>
+  </si>
+  <si>
+    <t>22nH SMD 1206 Inductor</t>
+  </si>
+  <si>
+    <t>815-AISC-1206-22NJ-T</t>
   </si>
 </sst>
 </file>
@@ -1362,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1540,7 +1540,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1554,7 +1554,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1607,13 +1607,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1663,13 +1663,13 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1691,13 +1691,13 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1719,13 +1719,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1761,10 +1761,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1831,7 +1831,7 @@
         <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
         <v>105</v>
@@ -1845,7 +1845,7 @@
         <v>127</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>126</v>
@@ -1859,10 +1859,10 @@
         <v>103</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1873,7 +1873,7 @@
         <v>125</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>124</v>
@@ -1884,13 +1884,13 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>